<commit_message>
product of array self-revise
</commit_message>
<xml_diff>
--- a/NeetCode 150.xlsx
+++ b/NeetCode 150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC239E25-0929-D647-8C15-A30D0D3C6BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C31361-8CE6-764F-953C-501CCA2A14E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="29920" windowHeight="18780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="328">
   <si>
     <t>Category</t>
   </si>
@@ -1671,7 +1671,9 @@
       <c r="B6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="13"/>
+      <c r="C6" s="13" t="s">
+        <v>327</v>
+      </c>
       <c r="D6" s="14" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
alien dict lc premium
</commit_message>
<xml_diff>
--- a/NeetCode 150.xlsx
+++ b/NeetCode 150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC26DB93-60CA-B543-828C-16D8954D2269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29520D18-C12C-FD41-A175-91E4320AFE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="23360" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="328">
   <si>
     <t>Category</t>
   </si>
@@ -1007,6 +1007,9 @@
   </si>
   <si>
     <t>Revised</t>
+  </si>
+  <si>
+    <t>Read</t>
   </si>
 </sst>
 </file>
@@ -1457,8 +1460,8 @@
   </sheetPr>
   <dimension ref="A1:AA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4872,7 +4875,9 @@
       <c r="B98" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="C98" s="13"/>
+      <c r="C98" s="13" t="s">
+        <v>327</v>
+      </c>
       <c r="D98" s="14" t="s">
         <v>213</v>
       </c>

</xml_diff>

<commit_message>
container w most water
</commit_message>
<xml_diff>
--- a/NeetCode 150.xlsx
+++ b/NeetCode 150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98E36ED-5866-F641-84B3-6984EF58CC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFFDD8F-47DB-7140-90AD-AD6A25924070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="23360" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="328">
   <si>
     <t>Category</t>
   </si>
@@ -1460,8 +1460,8 @@
   </sheetPr>
   <dimension ref="A1:AA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1957,7 +1957,9 @@
       <c r="B14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="20" t="s">
+        <v>326</v>
+      </c>
       <c r="D14" s="21" t="s">
         <v>35</v>
       </c>
@@ -3302,7 +3304,9 @@
       <c r="B53" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C53" s="13"/>
+      <c r="C53" s="13" t="s">
+        <v>326</v>
+      </c>
       <c r="D53" s="14" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
heap merge k lists
</commit_message>
<xml_diff>
--- a/NeetCode 150.xlsx
+++ b/NeetCode 150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFFDD8F-47DB-7140-90AD-AD6A25924070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F4D43E-71B4-BB41-A072-FDDDC3A589F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="23360" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="328">
   <si>
     <t>Category</t>
   </si>
@@ -1460,8 +1460,8 @@
   </sheetPr>
   <dimension ref="A1:AA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -3012,7 +3012,9 @@
       <c r="B45" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C45" s="13"/>
+      <c r="C45" s="13" t="s">
+        <v>326</v>
+      </c>
       <c r="D45" s="14" t="s">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
add two nums ll
</commit_message>
<xml_diff>
--- a/NeetCode 150.xlsx
+++ b/NeetCode 150.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F4D43E-71B4-BB41-A072-FDDDC3A589F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CDADF3-FABA-774E-A5B6-28A19A469C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="23360" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="23360" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Neetcode List" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="328">
   <si>
     <t>Category</t>
   </si>
@@ -1460,8 +1460,8 @@
   </sheetPr>
   <dimension ref="A1:AA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2800,7 +2800,9 @@
       <c r="B39" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="13"/>
+      <c r="C39" s="13" t="s">
+        <v>326</v>
+      </c>
       <c r="D39" s="14" t="s">
         <v>89</v>
       </c>
@@ -2870,7 +2872,9 @@
       <c r="B41" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="13"/>
+      <c r="C41" s="13" t="s">
+        <v>326</v>
+      </c>
       <c r="D41" s="14" t="s">
         <v>93</v>
       </c>
@@ -2942,7 +2946,9 @@
       <c r="B43" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C43" s="13"/>
+      <c r="C43" s="13" t="s">
+        <v>326</v>
+      </c>
       <c r="D43" s="14" t="s">
         <v>97</v>
       </c>

</xml_diff>